<commit_message>
replace default data with geopagackes
</commit_message>
<xml_diff>
--- a/test_data/swmm_data/gisswmm_transects.xlsx
+++ b/test_data/swmm_data/gisswmm_transects.xlsx
@@ -487,45 +487,29 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0.043</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.043</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0.043</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B2" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -534,45 +518,29 @@
           <t>tr_2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0.044000000000000004</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.043</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0.046</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B3" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -617,15 +585,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2.29</t>
-        </is>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.29</v>
       </c>
     </row>
     <row r="3">
@@ -634,15 +598,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2.22</t>
-        </is>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.22</v>
       </c>
     </row>
     <row r="4">
@@ -651,15 +611,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2.15</t>
-        </is>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.15</v>
       </c>
     </row>
     <row r="5">
@@ -668,15 +624,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2.09</t>
-        </is>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2.09</v>
       </c>
     </row>
     <row r="6">
@@ -685,15 +637,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2.01</t>
-        </is>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2.01</v>
       </c>
     </row>
     <row r="7">
@@ -702,15 +650,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>6.0</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1.92</t>
-        </is>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.92</v>
       </c>
     </row>
     <row r="8">
@@ -719,15 +663,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>7.0</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1.81</t>
-        </is>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.81</v>
       </c>
     </row>
     <row r="9">
@@ -736,15 +676,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>8.0</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1.7</t>
-        </is>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row r="10">
@@ -753,15 +689,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>9.0</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1.6</t>
-        </is>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.6</v>
       </c>
     </row>
     <row r="11">
@@ -770,15 +702,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>10.0</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1.52</t>
-        </is>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.52</v>
       </c>
     </row>
     <row r="12">
@@ -787,15 +715,11 @@
           <t>tr_1</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>11.0</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1.45</t>
-        </is>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.45</v>
       </c>
     </row>
     <row r="13">
@@ -804,15 +728,11 @@
           <t>tr_2</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>6.0</t>
-        </is>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -821,15 +741,11 @@
           <t>tr_2</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1.5</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>5.5</t>
-        </is>
+      <c r="B14" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5.5</v>
       </c>
     </row>
     <row r="15">
@@ -838,15 +754,11 @@
           <t>tr_2</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -855,15 +767,11 @@
           <t>tr_2</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>2.5</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>5.8</t>
-        </is>
+      <c r="B16" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>5.8</v>
       </c>
     </row>
     <row r="17">
@@ -872,15 +780,11 @@
           <t>tr_2</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>6.2</t>
-        </is>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" t="n">
+        <v>6.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>